<commit_message>
Test Case Final Updated
</commit_message>
<xml_diff>
--- a/Document/Test Case Pra UAS/Test Case Login Screen.xlsx
+++ b/Document/Test Case Pra UAS/Test Case Login Screen.xlsx
@@ -1,18 +1,86 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="19920" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="21">
+  <si>
+    <t>hasil</t>
+  </si>
+  <si>
+    <t>berhasil login</t>
+  </si>
+  <si>
+    <t>halaman login</t>
+  </si>
+  <si>
+    <t>form username untuk login</t>
+  </si>
+  <si>
+    <t>form password login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form username register </t>
+  </si>
+  <si>
+    <t>form kata sandi register</t>
+  </si>
+  <si>
+    <t>form konfirmasi kata sandi register</t>
+  </si>
+  <si>
+    <t>button login</t>
+  </si>
+  <si>
+    <t>button register</t>
+  </si>
+  <si>
+    <t>gagal login karena salah password</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>gagal login karena salah username(password diabaikan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gagal register karena username sudah ada yang pakai </t>
+  </si>
+  <si>
+    <t>gagal login karena username dan password login tidak di isi</t>
+  </si>
+  <si>
+    <t>gagal register karena password lebih dari 20 karakter</t>
+  </si>
+  <si>
+    <t>gagal register karena username lebih dari 30 karakter</t>
+  </si>
+  <si>
+    <t>gagal register karena konfirmasi password tidak match</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>gagal register karena form tidak di isi</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27,15 +95,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -43,18 +117,150 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,12 +549,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="65.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="62.25" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>